<commit_message>
fixed issue for  donors with same giftids
</commit_message>
<xml_diff>
--- a/public/Brick Layout Excel.xlsx
+++ b/public/Brick Layout Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbright\NATIONAL WESTERN STOCK SHOW\NATIONAL WESTERN STOCK SHOW Team Site - Documents\810 - Capital Fund Raising Campaign\Donor Approvals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NW26\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{536DBB36-D77B-4952-9901-E061BB2FF90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BAD1AE1-B479-4546-9944-D6628087DE8F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B6F47E-89B0-4AB9-8846-5281BBC68A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{AB601537-9FF5-466A-95DA-BA20506F4E27}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{AB601537-9FF5-466A-95DA-BA20506F4E27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t>A</t>
   </si>
@@ -372,16 +371,13 @@
   </si>
   <si>
     <t>TT</t>
-  </si>
-  <si>
-    <t>Final: 7/2/25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -804,3393 +800,3386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734CFBE6-C058-490A-85C9-DFD309FF7EAB}">
-  <dimension ref="A1:AI55"/>
+  <dimension ref="A1:AI47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
-    <col min="17" max="24" width="12.7109375" customWidth="1"/>
-    <col min="25" max="25" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" customWidth="1"/>
-    <col min="27" max="29" width="12.7109375" customWidth="1"/>
-    <col min="30" max="30" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="35" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" customWidth="1"/>
+    <col min="17" max="24" width="12.6640625" customWidth="1"/>
+    <col min="25" max="25" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5546875" customWidth="1"/>
+    <col min="27" max="29" width="12.6640625" customWidth="1"/>
+    <col min="30" max="30" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="35" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="12.75" customHeight="1"/>
-    <row r="2" spans="1:35" ht="9" customHeight="1"/>
-    <row r="3" spans="1:35" s="2" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2">
+    <row r="1" spans="1:35" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C1" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D1" s="2">
         <v>3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E1" s="2">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F1" s="2">
         <v>5</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G1" s="2">
         <v>6</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H1" s="2">
         <v>7</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I1" s="2">
         <v>8</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J1" s="2">
         <v>9</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K1" s="2">
         <v>10</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L1" s="2">
         <v>11</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M1" s="2">
         <v>12</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N1" s="2">
         <v>13</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O1" s="2">
         <v>14</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P1" s="2">
         <v>15</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q1" s="2">
         <v>16</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R1" s="2">
         <v>17</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S1" s="2">
         <v>18</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T1" s="2">
         <v>19</v>
       </c>
-      <c r="U3" s="2">
+      <c r="U1" s="2">
         <v>20</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V1" s="2">
         <v>21</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W1" s="2">
         <v>22</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X1" s="2">
         <v>23</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Y1" s="2">
         <v>24</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Z1" s="2">
         <v>25</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA1" s="2">
         <v>26</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AB1" s="2">
         <v>27</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AC1" s="2">
         <v>28</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AD1" s="2">
         <v>29</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AE1" s="2">
         <v>30</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AF1" s="2">
         <v>31</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AG1" s="2">
         <v>32</v>
       </c>
-      <c r="AH3" s="2">
+      <c r="AH1" s="2">
         <v>33</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AI1" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="25.15" customHeight="1">
+    <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="4"/>
+    </row>
+    <row r="3" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="3"/>
+    </row>
+    <row r="4" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2436</v>
+      </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="5">
+        <v>212</v>
+      </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="5">
+        <v>2437</v>
+      </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="3"/>
+      <c r="H4" s="5">
+        <v>2438</v>
+      </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="5">
+        <v>1435</v>
+      </c>
       <c r="K4" s="4"/>
-      <c r="L4" s="3"/>
+      <c r="L4" s="5">
+        <v>753</v>
+      </c>
       <c r="M4" s="4"/>
-      <c r="N4" s="3"/>
+      <c r="N4" s="5">
+        <v>752</v>
+      </c>
       <c r="O4" s="4"/>
-      <c r="P4" s="3"/>
+      <c r="P4" s="5">
+        <v>192</v>
+      </c>
       <c r="Q4" s="4"/>
-      <c r="R4" s="3"/>
+      <c r="R4" s="5">
+        <v>921</v>
+      </c>
       <c r="S4" s="4"/>
-      <c r="T4" s="3"/>
+      <c r="T4" s="5">
+        <v>2629</v>
+      </c>
       <c r="U4" s="4"/>
-      <c r="V4" s="3"/>
+      <c r="V4" s="5">
+        <v>2530</v>
+      </c>
       <c r="W4" s="4"/>
-      <c r="X4" s="3"/>
+      <c r="X4" s="5">
+        <v>931</v>
+      </c>
       <c r="Y4" s="4"/>
-      <c r="Z4" s="3"/>
+      <c r="Z4" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="AA4" s="4"/>
-      <c r="AB4" s="3"/>
+      <c r="AB4" s="5">
+        <v>291</v>
+      </c>
       <c r="AC4" s="4"/>
-      <c r="AD4" s="3"/>
+      <c r="AD4" s="5">
+        <v>641</v>
+      </c>
       <c r="AE4" s="4"/>
-      <c r="AF4" s="3"/>
+      <c r="AF4" s="5">
+        <v>293</v>
+      </c>
       <c r="AG4" s="4"/>
-      <c r="AH4" s="3"/>
+      <c r="AH4" s="5">
+        <v>2283</v>
+      </c>
       <c r="AI4" s="4"/>
     </row>
-    <row r="5" spans="1:35" ht="25.15" customHeight="1">
+    <row r="5" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="5">
+        <v>564</v>
+      </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="5">
+        <v>1867</v>
+      </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="5">
+        <v>2439</v>
+      </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="5">
+        <v>886</v>
+      </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="3"/>
+      <c r="K5" s="5">
+        <v>580</v>
+      </c>
       <c r="L5" s="4"/>
-      <c r="M5" s="3"/>
+      <c r="M5" s="5">
+        <v>57</v>
+      </c>
       <c r="N5" s="4"/>
-      <c r="O5" s="3"/>
+      <c r="O5" s="5">
+        <v>1568</v>
+      </c>
       <c r="P5" s="4"/>
-      <c r="Q5" s="3"/>
+      <c r="Q5" s="5">
+        <v>2193</v>
+      </c>
       <c r="R5" s="4"/>
-      <c r="S5" s="3"/>
+      <c r="S5" s="5">
+        <v>2226</v>
+      </c>
       <c r="T5" s="4"/>
-      <c r="U5" s="3"/>
+      <c r="U5" s="5">
+        <v>581</v>
+      </c>
       <c r="V5" s="4"/>
-      <c r="W5" s="3"/>
+      <c r="W5" s="5">
+        <v>2622</v>
+      </c>
       <c r="X5" s="4"/>
-      <c r="Y5" s="3"/>
+      <c r="Y5" s="5">
+        <v>1449</v>
+      </c>
       <c r="Z5" s="4"/>
-      <c r="AA5" s="3"/>
+      <c r="AA5" s="5">
+        <v>391</v>
+      </c>
       <c r="AB5" s="4"/>
-      <c r="AC5" s="3"/>
+      <c r="AC5" s="5">
+        <v>247</v>
+      </c>
       <c r="AD5" s="4"/>
-      <c r="AE5" s="3"/>
+      <c r="AE5" s="5">
+        <v>2373</v>
+      </c>
       <c r="AF5" s="4"/>
-      <c r="AG5" s="3"/>
+      <c r="AG5" s="5">
+        <v>2659</v>
+      </c>
       <c r="AH5" s="4"/>
-      <c r="AI5" s="3"/>
-    </row>
-    <row r="6" spans="1:35" ht="25.15" customHeight="1">
+      <c r="AI5" s="5">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>2436</v>
+        <v>685</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5">
-        <v>212</v>
+        <v>2405</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5">
-        <v>2437</v>
+        <v>1158</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="5">
-        <v>2438</v>
+        <v>2381</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="5">
-        <v>1435</v>
+        <v>935</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="5">
-        <v>753</v>
+        <v>2628</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="5">
-        <v>752</v>
+        <v>156</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="5">
-        <v>192</v>
+        <v>2581</v>
       </c>
       <c r="Q6" s="4"/>
-      <c r="R6" s="5">
-        <v>921</v>
+      <c r="R6" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="S6" s="4"/>
       <c r="T6" s="5">
-        <v>2629</v>
+        <v>341</v>
       </c>
       <c r="U6" s="4"/>
       <c r="V6" s="5">
-        <v>2530</v>
+        <v>996</v>
       </c>
       <c r="W6" s="4"/>
       <c r="X6" s="5">
-        <v>931</v>
+        <v>578</v>
       </c>
       <c r="Y6" s="4"/>
-      <c r="Z6" s="5" t="s">
-        <v>3</v>
+      <c r="Z6" s="5">
+        <v>782</v>
       </c>
       <c r="AA6" s="4"/>
       <c r="AB6" s="5">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="AC6" s="4"/>
       <c r="AD6" s="5">
-        <v>641</v>
+        <v>340</v>
       </c>
       <c r="AE6" s="4"/>
       <c r="AF6" s="5">
-        <v>293</v>
+        <v>2376</v>
       </c>
       <c r="AG6" s="4"/>
       <c r="AH6" s="5">
-        <v>2283</v>
+        <v>977</v>
       </c>
       <c r="AI6" s="4"/>
     </row>
-    <row r="7" spans="1:35" ht="25.15" customHeight="1">
+    <row r="7" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5">
-        <v>564</v>
+        <v>2389</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="5">
-        <v>1867</v>
+      <c r="E7" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5">
-        <v>2439</v>
+        <v>2327</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="5">
-        <v>886</v>
+        <v>2328</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="5">
-        <v>580</v>
+        <v>2391</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="5">
-        <v>57</v>
+        <v>2516</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="5">
-        <v>1568</v>
+        <v>1202</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="5">
-        <v>2193</v>
+        <v>1203</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="5">
-        <v>2226</v>
+        <v>2227</v>
       </c>
       <c r="T7" s="4"/>
       <c r="U7" s="5">
-        <v>581</v>
+        <v>314</v>
       </c>
       <c r="V7" s="4"/>
       <c r="W7" s="5">
-        <v>2622</v>
+        <v>2589</v>
       </c>
       <c r="X7" s="4"/>
       <c r="Y7" s="5">
-        <v>1449</v>
+        <v>573</v>
       </c>
       <c r="Z7" s="4"/>
       <c r="AA7" s="5">
-        <v>391</v>
+        <v>1644</v>
       </c>
       <c r="AB7" s="4"/>
       <c r="AC7" s="5">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="AD7" s="4"/>
-      <c r="AE7" s="5">
-        <v>2373</v>
+      <c r="AE7" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="AF7" s="4"/>
       <c r="AG7" s="5">
-        <v>2659</v>
+        <v>569</v>
       </c>
       <c r="AH7" s="4"/>
       <c r="AI7" s="5">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" ht="25.15" customHeight="1">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5">
-        <v>685</v>
+        <v>213</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5">
-        <v>2405</v>
+        <v>891</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="5">
-        <v>1158</v>
+        <v>2645</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="5">
-        <v>2381</v>
+        <v>474</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="5">
-        <v>935</v>
+        <v>335</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="5">
-        <v>2628</v>
+        <v>2442</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="5">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="5">
-        <v>2581</v>
+        <v>1505</v>
       </c>
       <c r="Q8" s="4"/>
-      <c r="R8" s="5" t="s">
-        <v>6</v>
+      <c r="R8" s="5">
+        <v>2457</v>
       </c>
       <c r="S8" s="4"/>
       <c r="T8" s="5">
-        <v>341</v>
+        <v>1637</v>
       </c>
       <c r="U8" s="4"/>
       <c r="V8" s="5">
-        <v>996</v>
+        <v>160</v>
       </c>
       <c r="W8" s="4"/>
       <c r="X8" s="5">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="Y8" s="4"/>
       <c r="Z8" s="5">
-        <v>782</v>
+        <v>193</v>
       </c>
       <c r="AA8" s="4"/>
       <c r="AB8" s="5">
-        <v>277</v>
+        <v>2621</v>
       </c>
       <c r="AC8" s="4"/>
       <c r="AD8" s="5">
-        <v>340</v>
+        <v>1920</v>
       </c>
       <c r="AE8" s="4"/>
       <c r="AF8" s="5">
-        <v>2376</v>
+        <v>954</v>
       </c>
       <c r="AG8" s="4"/>
       <c r="AH8" s="5">
-        <v>977</v>
+        <v>250</v>
       </c>
       <c r="AI8" s="4"/>
     </row>
-    <row r="9" spans="1:35" ht="25.15" customHeight="1">
+    <row r="9" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5">
-        <v>2389</v>
+        <v>2674</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="5" t="s">
-        <v>8</v>
+      <c r="E9" s="5">
+        <v>2603</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="5">
-        <v>2327</v>
+        <v>686</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="5">
-        <v>2328</v>
+        <v>23</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="5">
-        <v>2391</v>
+        <v>806</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="5">
-        <v>2516</v>
+        <v>459</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="5">
-        <v>1202</v>
+        <v>351</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="5">
-        <v>1203</v>
+        <v>352</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="5">
-        <v>2227</v>
+        <v>658</v>
       </c>
       <c r="T9" s="4"/>
       <c r="U9" s="5">
-        <v>314</v>
+        <v>1652</v>
       </c>
       <c r="V9" s="4"/>
       <c r="W9" s="5">
-        <v>2589</v>
+        <v>1528</v>
       </c>
       <c r="X9" s="4"/>
       <c r="Y9" s="5">
-        <v>573</v>
+        <v>2637</v>
       </c>
       <c r="Z9" s="4"/>
       <c r="AA9" s="5">
-        <v>1644</v>
+        <v>483</v>
       </c>
       <c r="AB9" s="4"/>
       <c r="AC9" s="5">
-        <v>311</v>
+        <v>14</v>
       </c>
       <c r="AD9" s="4"/>
-      <c r="AE9" s="5" t="s">
-        <v>9</v>
+      <c r="AE9" s="5">
+        <v>938</v>
       </c>
       <c r="AF9" s="4"/>
       <c r="AG9" s="5">
-        <v>569</v>
+        <v>923</v>
       </c>
       <c r="AH9" s="4"/>
       <c r="AI9" s="5">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" ht="25.15" customHeight="1">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5">
-        <v>213</v>
+        <v>1060</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5">
-        <v>891</v>
+        <v>1061</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="5">
-        <v>2645</v>
+        <v>312</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="5">
-        <v>474</v>
+        <v>2434</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="5">
-        <v>335</v>
+        <v>2452</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="5">
-        <v>2442</v>
+        <v>2448</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="5">
-        <v>182</v>
+        <v>2665</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="5">
-        <v>1505</v>
+        <v>1393</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="5">
-        <v>2457</v>
+        <v>2359</v>
       </c>
       <c r="S10" s="4"/>
       <c r="T10" s="5">
-        <v>1637</v>
+        <v>1204</v>
       </c>
       <c r="U10" s="4"/>
       <c r="V10" s="5">
-        <v>160</v>
+        <v>375</v>
       </c>
       <c r="W10" s="4"/>
       <c r="X10" s="5">
-        <v>582</v>
+        <v>565</v>
       </c>
       <c r="Y10" s="4"/>
       <c r="Z10" s="5">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="AA10" s="4"/>
-      <c r="AB10" s="5">
-        <v>2621</v>
+      <c r="AB10" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="AC10" s="4"/>
       <c r="AD10" s="5">
-        <v>1920</v>
+        <v>167</v>
       </c>
       <c r="AE10" s="4"/>
       <c r="AF10" s="5">
-        <v>954</v>
+        <v>165</v>
       </c>
       <c r="AG10" s="4"/>
       <c r="AH10" s="5">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="AI10" s="4"/>
     </row>
-    <row r="11" spans="1:35" ht="25.15" customHeight="1">
+    <row r="11" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="5">
-        <v>2674</v>
+        <v>951</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="5">
-        <v>2603</v>
+        <v>952</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="5">
-        <v>686</v>
+        <v>1532</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="5">
-        <v>23</v>
+        <v>2601</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="5">
-        <v>806</v>
+        <v>216</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="5">
-        <v>459</v>
+        <v>438</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="5">
-        <v>351</v>
+        <v>20</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="5">
-        <v>352</v>
+        <v>1195</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="5">
-        <v>658</v>
+        <v>2685</v>
       </c>
       <c r="T11" s="4"/>
       <c r="U11" s="5">
-        <v>1652</v>
+        <v>2686</v>
       </c>
       <c r="V11" s="4"/>
       <c r="W11" s="5">
-        <v>1528</v>
+        <v>1531</v>
       </c>
       <c r="X11" s="4"/>
       <c r="Y11" s="5">
-        <v>2637</v>
+        <v>2512</v>
       </c>
       <c r="Z11" s="4"/>
       <c r="AA11" s="5">
-        <v>483</v>
+        <v>2384</v>
       </c>
       <c r="AB11" s="4"/>
       <c r="AC11" s="5">
-        <v>14</v>
+        <v>430</v>
       </c>
       <c r="AD11" s="4"/>
-      <c r="AE11" s="5">
-        <v>938</v>
+      <c r="AE11" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="AF11" s="4"/>
       <c r="AG11" s="5">
-        <v>923</v>
+        <v>204</v>
       </c>
       <c r="AH11" s="4"/>
       <c r="AI11" s="5">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" ht="25.15" customHeight="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5">
-        <v>1060</v>
+        <v>233</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5">
-        <v>1061</v>
+        <v>244</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="5">
-        <v>312</v>
+        <v>587</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5">
-        <v>2434</v>
+        <v>1466</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="5">
-        <v>2452</v>
+        <v>496</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="5">
-        <v>2448</v>
+        <v>448</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="5">
-        <v>2665</v>
+        <v>1058</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="5">
-        <v>1393</v>
+        <v>1059</v>
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="5">
-        <v>2359</v>
+        <v>2625</v>
       </c>
       <c r="S12" s="4"/>
       <c r="T12" s="5">
-        <v>1204</v>
+        <v>2687</v>
       </c>
       <c r="U12" s="4"/>
       <c r="V12" s="5">
-        <v>375</v>
+        <v>342</v>
       </c>
       <c r="W12" s="4"/>
       <c r="X12" s="5">
-        <v>565</v>
+        <v>366</v>
       </c>
       <c r="Y12" s="4"/>
-      <c r="Z12" s="5">
-        <v>227</v>
+      <c r="Z12" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="AA12" s="4"/>
-      <c r="AB12" s="5" t="s">
-        <v>13</v>
+      <c r="AB12" s="5">
+        <v>560</v>
       </c>
       <c r="AC12" s="4"/>
       <c r="AD12" s="5">
-        <v>167</v>
+        <v>1183</v>
       </c>
       <c r="AE12" s="4"/>
       <c r="AF12" s="5">
-        <v>165</v>
+        <v>2341</v>
       </c>
       <c r="AG12" s="4"/>
       <c r="AH12" s="5">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="AI12" s="4"/>
     </row>
-    <row r="13" spans="1:35" ht="25.15" customHeight="1">
+    <row r="13" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="5">
-        <v>951</v>
+        <v>1065</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="5">
-        <v>952</v>
+        <v>1064</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="5">
-        <v>1532</v>
+        <v>181</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="5">
-        <v>2601</v>
+        <v>2238</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="5">
-        <v>216</v>
+        <v>431</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="5">
-        <v>438</v>
+        <v>1453</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="5">
-        <v>20</v>
+        <v>554</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="5">
-        <v>1195</v>
+        <v>583</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="5">
-        <v>2685</v>
+        <v>859</v>
       </c>
       <c r="T13" s="4"/>
       <c r="U13" s="5">
-        <v>2686</v>
+        <v>434</v>
       </c>
       <c r="V13" s="4"/>
       <c r="W13" s="5">
-        <v>1531</v>
+        <v>2487</v>
       </c>
       <c r="X13" s="4"/>
       <c r="Y13" s="5">
-        <v>2512</v>
+        <v>2626</v>
       </c>
       <c r="Z13" s="4"/>
       <c r="AA13" s="5">
-        <v>2384</v>
+        <v>2390</v>
       </c>
       <c r="AB13" s="4"/>
       <c r="AC13" s="5">
-        <v>430</v>
+        <v>937</v>
       </c>
       <c r="AD13" s="4"/>
-      <c r="AE13" s="5" t="s">
-        <v>15</v>
+      <c r="AE13" s="5">
+        <v>1166</v>
       </c>
       <c r="AF13" s="4"/>
       <c r="AG13" s="5">
-        <v>204</v>
+        <v>833</v>
       </c>
       <c r="AH13" s="4"/>
       <c r="AI13" s="5">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" ht="25.15" customHeight="1">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5">
-        <v>233</v>
+        <v>19</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="5">
-        <v>244</v>
+        <v>767</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="5">
-        <v>587</v>
+      <c r="F14" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="5">
-        <v>1466</v>
+      <c r="H14" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="J14" s="5">
-        <v>496</v>
+      <c r="J14" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="5">
-        <v>448</v>
+        <v>1831</v>
       </c>
       <c r="M14" s="4"/>
-      <c r="N14" s="5">
-        <v>1058</v>
+      <c r="N14" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="5">
-        <v>1059</v>
+        <v>1070</v>
       </c>
       <c r="Q14" s="4"/>
       <c r="R14" s="5">
-        <v>2625</v>
+        <v>1071</v>
       </c>
       <c r="S14" s="4"/>
-      <c r="T14" s="5">
-        <v>2687</v>
+      <c r="T14" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="U14" s="4"/>
       <c r="V14" s="5">
-        <v>342</v>
+        <v>1082</v>
       </c>
       <c r="W14" s="4"/>
       <c r="X14" s="5">
-        <v>366</v>
+        <v>1083</v>
       </c>
       <c r="Y14" s="4"/>
       <c r="Z14" s="5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="AA14" s="4"/>
       <c r="AB14" s="5">
-        <v>560</v>
+        <v>2496</v>
       </c>
       <c r="AC14" s="4"/>
       <c r="AD14" s="5">
-        <v>1183</v>
+        <v>2616</v>
       </c>
       <c r="AE14" s="4"/>
       <c r="AF14" s="5">
-        <v>2341</v>
+        <v>2537</v>
       </c>
       <c r="AG14" s="4"/>
       <c r="AH14" s="5">
-        <v>148</v>
+        <v>330</v>
       </c>
       <c r="AI14" s="4"/>
     </row>
-    <row r="15" spans="1:35" ht="25.15" customHeight="1">
+    <row r="15" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="5">
-        <v>1065</v>
+        <v>70</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="5">
-        <v>1064</v>
+        <v>1207</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="5">
-        <v>181</v>
+        <v>990</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="5">
-        <v>2238</v>
+        <v>989</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="5">
-        <v>431</v>
+        <v>1915</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="5">
-        <v>1453</v>
+        <v>899</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="5">
-        <v>554</v>
+        <v>898</v>
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="5">
-        <v>583</v>
+        <v>2502</v>
       </c>
       <c r="R15" s="4"/>
-      <c r="S15" s="5">
-        <v>859</v>
+      <c r="S15" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="T15" s="4"/>
-      <c r="U15" s="5">
-        <v>434</v>
+      <c r="U15" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="V15" s="4"/>
       <c r="W15" s="5">
-        <v>2487</v>
+        <v>660</v>
       </c>
       <c r="X15" s="4"/>
       <c r="Y15" s="5">
-        <v>2626</v>
+        <v>2627</v>
       </c>
       <c r="Z15" s="4"/>
       <c r="AA15" s="5">
-        <v>2390</v>
+        <v>2650</v>
       </c>
       <c r="AB15" s="4"/>
       <c r="AC15" s="5">
-        <v>937</v>
+        <v>2055</v>
       </c>
       <c r="AD15" s="4"/>
       <c r="AE15" s="5">
-        <v>1166</v>
+        <v>2762</v>
       </c>
       <c r="AF15" s="4"/>
       <c r="AG15" s="5">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="AH15" s="4"/>
       <c r="AI15" s="5">
-        <v>1205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:35" ht="25.15" customHeight="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B16" s="5">
+        <v>650</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="5">
-        <v>767</v>
+        <v>2584</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="5" t="s">
-        <v>21</v>
+      <c r="F16" s="5">
+        <v>2233</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="5" t="s">
-        <v>22</v>
+      <c r="H16" s="5">
+        <v>991</v>
       </c>
       <c r="I16" s="4"/>
-      <c r="J16" s="5" t="s">
-        <v>23</v>
+      <c r="J16" s="5">
+        <v>1911</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="5">
-        <v>1831</v>
+        <v>897</v>
       </c>
       <c r="M16" s="4"/>
-      <c r="N16" s="5" t="s">
-        <v>24</v>
+      <c r="N16" s="5">
+        <v>896</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="5">
-        <v>1070</v>
+        <v>902</v>
       </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="5">
-        <v>1071</v>
+        <v>276</v>
       </c>
       <c r="S16" s="4"/>
       <c r="T16" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="U16" s="4"/>
       <c r="V16" s="5">
-        <v>1082</v>
+        <v>1838</v>
       </c>
       <c r="W16" s="4"/>
       <c r="X16" s="5">
-        <v>1083</v>
+        <v>1217</v>
       </c>
       <c r="Y16" s="4"/>
-      <c r="Z16" s="5" t="s">
-        <v>26</v>
+      <c r="Z16" s="5">
+        <v>568</v>
       </c>
       <c r="AA16" s="4"/>
       <c r="AB16" s="5">
-        <v>2496</v>
+        <v>2497</v>
       </c>
       <c r="AC16" s="4"/>
       <c r="AD16" s="5">
-        <v>2616</v>
+        <v>2612</v>
       </c>
       <c r="AE16" s="4"/>
       <c r="AF16" s="5">
-        <v>2537</v>
+        <v>684</v>
       </c>
       <c r="AG16" s="4"/>
       <c r="AH16" s="5">
-        <v>330</v>
+        <v>424</v>
       </c>
       <c r="AI16" s="4"/>
     </row>
-    <row r="17" spans="1:35" ht="25.15" customHeight="1">
+    <row r="17" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="5">
-        <v>70</v>
+        <v>2583</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="5">
-        <v>1207</v>
+        <v>2586</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="5">
-        <v>990</v>
+        <v>1910</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="5">
-        <v>989</v>
+        <v>1909</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="5">
-        <v>1915</v>
+        <v>1916</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="5">
-        <v>899</v>
+        <v>2636</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="5">
-        <v>898</v>
+        <v>2235</v>
       </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="5">
-        <v>2502</v>
+        <v>2236</v>
       </c>
       <c r="R17" s="4"/>
-      <c r="S17" s="5" t="s">
-        <v>28</v>
+      <c r="S17" s="5">
+        <v>2237</v>
       </c>
       <c r="T17" s="4"/>
-      <c r="U17" s="5" t="s">
-        <v>29</v>
+      <c r="U17" s="5">
+        <v>657</v>
       </c>
       <c r="V17" s="4"/>
       <c r="W17" s="5">
-        <v>660</v>
+        <v>2154</v>
       </c>
       <c r="X17" s="4"/>
       <c r="Y17" s="5">
-        <v>2627</v>
+        <v>220</v>
       </c>
       <c r="Z17" s="4"/>
       <c r="AA17" s="5">
-        <v>2650</v>
+        <v>715</v>
       </c>
       <c r="AB17" s="4"/>
       <c r="AC17" s="5">
-        <v>2055</v>
+        <v>716</v>
       </c>
       <c r="AD17" s="4"/>
       <c r="AE17" s="5">
-        <v>2762</v>
+        <v>1078</v>
       </c>
       <c r="AF17" s="4"/>
       <c r="AG17" s="5">
-        <v>836</v>
+        <v>1079</v>
       </c>
       <c r="AH17" s="4"/>
       <c r="AI17" s="5">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35" ht="25.15" customHeight="1">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B18" s="5">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="5">
-        <v>2584</v>
+        <v>2587</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="5">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="5">
-        <v>991</v>
+        <v>2231</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="5">
-        <v>1911</v>
+        <v>1912</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="5">
-        <v>897</v>
+        <v>2482</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="5">
-        <v>896</v>
+        <v>2348</v>
       </c>
       <c r="O18" s="4"/>
-      <c r="P18" s="5">
-        <v>902</v>
+      <c r="P18" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="Q18" s="4"/>
       <c r="R18" s="5">
-        <v>276</v>
+        <v>927</v>
       </c>
       <c r="S18" s="4"/>
-      <c r="T18" s="5" t="s">
-        <v>31</v>
+      <c r="T18" s="5">
+        <v>2241</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="5">
-        <v>1838</v>
+        <v>1054</v>
       </c>
       <c r="W18" s="4"/>
       <c r="X18" s="5">
-        <v>1217</v>
+        <v>1055</v>
       </c>
       <c r="Y18" s="4"/>
       <c r="Z18" s="5">
-        <v>568</v>
+        <v>717</v>
       </c>
       <c r="AA18" s="4"/>
       <c r="AB18" s="5">
-        <v>2497</v>
+        <v>718</v>
       </c>
       <c r="AC18" s="4"/>
       <c r="AD18" s="5">
-        <v>2612</v>
+        <v>2385</v>
       </c>
       <c r="AE18" s="4"/>
       <c r="AF18" s="5">
-        <v>684</v>
+        <v>1174</v>
       </c>
       <c r="AG18" s="4"/>
       <c r="AH18" s="5">
-        <v>424</v>
+        <v>1151</v>
       </c>
       <c r="AI18" s="4"/>
     </row>
-    <row r="19" spans="1:35" ht="25.15" customHeight="1">
+    <row r="19" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="5">
-        <v>2583</v>
+        <v>2585</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="5">
-        <v>2586</v>
+        <v>339</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="5">
-        <v>1910</v>
+        <v>1913</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="5">
-        <v>1909</v>
+        <v>1914</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="5">
-        <v>1916</v>
+        <v>1917</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="5">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="5">
-        <v>2235</v>
+        <v>1419</v>
       </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="5">
-        <v>2236</v>
+        <v>2525</v>
       </c>
       <c r="R19" s="4"/>
       <c r="S19" s="5">
-        <v>2237</v>
+        <v>1859</v>
       </c>
       <c r="T19" s="4"/>
       <c r="U19" s="5">
-        <v>657</v>
+        <v>1150</v>
       </c>
       <c r="V19" s="4"/>
       <c r="W19" s="5">
-        <v>2154</v>
+        <v>1648</v>
       </c>
       <c r="X19" s="4"/>
       <c r="Y19" s="5">
-        <v>220</v>
+        <v>2484</v>
       </c>
       <c r="Z19" s="4"/>
       <c r="AA19" s="5">
-        <v>715</v>
+        <v>2485</v>
       </c>
       <c r="AB19" s="4"/>
-      <c r="AC19" s="5">
-        <v>716</v>
+      <c r="AC19" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="AD19" s="4"/>
-      <c r="AE19" s="5">
-        <v>1078</v>
+      <c r="AE19" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="AF19" s="4"/>
       <c r="AG19" s="5">
-        <v>1079</v>
+        <v>1003</v>
       </c>
       <c r="AH19" s="4"/>
       <c r="AI19" s="5">
-        <v>1175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" ht="25.15" customHeight="1">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B20" s="5">
-        <v>651</v>
+        <v>920</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5">
-        <v>2587</v>
+        <v>24</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="5">
-        <v>2232</v>
+        <v>2234</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="5">
-        <v>2231</v>
+        <v>224</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="5">
-        <v>1912</v>
+        <v>439</v>
       </c>
       <c r="K20" s="4"/>
-      <c r="L20" s="5">
-        <v>2482</v>
+      <c r="L20" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="5">
-        <v>2348</v>
+        <v>2404</v>
       </c>
       <c r="O20" s="4"/>
-      <c r="P20" s="5" t="s">
-        <v>34</v>
+      <c r="P20" s="5">
+        <v>2597</v>
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="5">
-        <v>927</v>
+        <v>2598</v>
       </c>
       <c r="S20" s="4"/>
       <c r="T20" s="5">
-        <v>2241</v>
+        <v>1629</v>
       </c>
       <c r="U20" s="4"/>
       <c r="V20" s="5">
-        <v>1054</v>
+        <v>2489</v>
       </c>
       <c r="W20" s="4"/>
       <c r="X20" s="5">
-        <v>1055</v>
+        <v>2393</v>
       </c>
       <c r="Y20" s="4"/>
       <c r="Z20" s="5">
-        <v>717</v>
+        <v>270</v>
       </c>
       <c r="AA20" s="4"/>
-      <c r="AB20" s="5">
-        <v>718</v>
+      <c r="AB20" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="AC20" s="4"/>
-      <c r="AD20" s="5">
-        <v>2385</v>
+      <c r="AD20" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="AE20" s="4"/>
       <c r="AF20" s="5">
-        <v>1174</v>
+        <v>1002</v>
       </c>
       <c r="AG20" s="4"/>
       <c r="AH20" s="5">
-        <v>1151</v>
+        <v>1000</v>
       </c>
       <c r="AI20" s="4"/>
     </row>
-    <row r="21" spans="1:35" ht="25.15" customHeight="1">
+    <row r="21" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="5">
-        <v>2585</v>
+        <v>2310</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="5">
-        <v>339</v>
+        <v>438</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="5">
-        <v>1913</v>
+        <v>1876</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="5">
-        <v>1914</v>
+        <v>1194</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="5">
-        <v>1917</v>
+        <v>2672</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="5">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="5">
-        <v>1419</v>
+        <v>2500</v>
       </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="5">
-        <v>2525</v>
+        <v>1627</v>
       </c>
       <c r="R21" s="4"/>
       <c r="S21" s="5">
-        <v>1859</v>
+        <v>1628</v>
       </c>
       <c r="T21" s="4"/>
       <c r="U21" s="5">
-        <v>1150</v>
+        <v>180</v>
       </c>
       <c r="V21" s="4"/>
-      <c r="W21" s="5">
-        <v>1648</v>
+      <c r="W21" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="X21" s="4"/>
       <c r="Y21" s="5">
-        <v>2484</v>
+        <v>2691</v>
       </c>
       <c r="Z21" s="4"/>
       <c r="AA21" s="5">
-        <v>2485</v>
+        <v>697</v>
       </c>
       <c r="AB21" s="4"/>
-      <c r="AC21" s="5" t="s">
-        <v>36</v>
+      <c r="AC21" s="5">
+        <v>2454</v>
       </c>
       <c r="AD21" s="4"/>
       <c r="AE21" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="AF21" s="4"/>
       <c r="AG21" s="5">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="AH21" s="4"/>
       <c r="AI21" s="5">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:35" ht="25.15" customHeight="1">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B22" s="5">
-        <v>920</v>
+        <v>2468</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="5">
-        <v>24</v>
+        <v>2469</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="5">
-        <v>2234</v>
+        <v>2471</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="5">
-        <v>224</v>
+        <v>2473</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="5">
-        <v>439</v>
+        <v>124</v>
       </c>
       <c r="K22" s="4"/>
-      <c r="L22" s="5" t="s">
-        <v>39</v>
+      <c r="L22" s="5">
+        <v>1898</v>
       </c>
       <c r="M22" s="4"/>
-      <c r="N22" s="5">
-        <v>2404</v>
+      <c r="N22" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="5">
-        <v>2597</v>
+        <v>2315</v>
       </c>
       <c r="Q22" s="4"/>
       <c r="R22" s="5">
-        <v>2598</v>
+        <v>2316</v>
       </c>
       <c r="S22" s="4"/>
       <c r="T22" s="5">
-        <v>1629</v>
+        <v>2317</v>
       </c>
       <c r="U22" s="4"/>
       <c r="V22" s="5">
-        <v>2489</v>
+        <v>402</v>
       </c>
       <c r="W22" s="4"/>
       <c r="X22" s="5">
-        <v>2393</v>
+        <v>1523</v>
       </c>
       <c r="Y22" s="4"/>
       <c r="Z22" s="5">
-        <v>270</v>
+        <v>1524</v>
       </c>
       <c r="AA22" s="4"/>
-      <c r="AB22" s="5" t="s">
-        <v>40</v>
+      <c r="AB22" s="5">
+        <v>2431</v>
       </c>
       <c r="AC22" s="4"/>
-      <c r="AD22" s="5" t="s">
-        <v>41</v>
+      <c r="AD22" s="5">
+        <v>2432</v>
       </c>
       <c r="AE22" s="4"/>
       <c r="AF22" s="5">
-        <v>1002</v>
+        <v>997</v>
       </c>
       <c r="AG22" s="4"/>
       <c r="AH22" s="5">
-        <v>1000</v>
+        <v>887</v>
       </c>
       <c r="AI22" s="4"/>
     </row>
-    <row r="23" spans="1:35" ht="25.15" customHeight="1">
+    <row r="23" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5">
-        <v>2310</v>
+        <v>1025</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="5">
-        <v>438</v>
+        <v>2470</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="5">
-        <v>1876</v>
+        <v>2472</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="5">
-        <v>1194</v>
+        <v>2421</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="5">
-        <v>2672</v>
+        <v>380</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="5">
-        <v>2634</v>
+        <v>721</v>
       </c>
       <c r="N23" s="4"/>
       <c r="O23" s="5">
-        <v>2500</v>
+        <v>1022</v>
       </c>
       <c r="P23" s="4"/>
-      <c r="Q23" s="5">
-        <v>1627</v>
+      <c r="Q23" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="R23" s="4"/>
       <c r="S23" s="5">
-        <v>1628</v>
+        <v>321</v>
       </c>
       <c r="T23" s="4"/>
       <c r="U23" s="5">
-        <v>180</v>
+        <v>586</v>
       </c>
       <c r="V23" s="4"/>
-      <c r="W23" s="5" t="s">
-        <v>43</v>
+      <c r="W23" s="5">
+        <v>2508</v>
       </c>
       <c r="X23" s="4"/>
-      <c r="Y23" s="5">
-        <v>2691</v>
+      <c r="Y23" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="Z23" s="4"/>
       <c r="AA23" s="5">
-        <v>697</v>
+        <v>703</v>
       </c>
       <c r="AB23" s="4"/>
       <c r="AC23" s="5">
-        <v>2454</v>
+        <v>411</v>
       </c>
       <c r="AD23" s="4"/>
-      <c r="AE23" s="5" t="s">
-        <v>44</v>
+      <c r="AE23" s="5">
+        <v>1801</v>
       </c>
       <c r="AF23" s="4"/>
       <c r="AG23" s="5">
-        <v>1004</v>
+        <v>1851</v>
       </c>
       <c r="AH23" s="4"/>
       <c r="AI23" s="5">
-        <v>2217</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" ht="25.15" customHeight="1">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B24" s="5">
-        <v>2468</v>
+        <v>1023</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="5">
-        <v>2469</v>
+        <v>1026</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="5">
-        <v>2471</v>
+        <v>1028</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="5">
-        <v>2473</v>
+        <v>1030</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="5">
-        <v>124</v>
+        <v>598</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="5">
-        <v>1898</v>
+        <v>1017</v>
       </c>
       <c r="M24" s="4"/>
-      <c r="N24" s="5" t="s">
-        <v>46</v>
+      <c r="N24" s="5">
+        <v>1021</v>
       </c>
       <c r="O24" s="4"/>
-      <c r="P24" s="5">
-        <v>2315</v>
+      <c r="P24" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="Q24" s="4"/>
       <c r="R24" s="5">
-        <v>2316</v>
+        <v>1008</v>
       </c>
       <c r="S24" s="4"/>
       <c r="T24" s="5">
-        <v>2317</v>
+        <v>1009</v>
       </c>
       <c r="U24" s="4"/>
       <c r="V24" s="5">
-        <v>402</v>
+        <v>2483</v>
       </c>
       <c r="W24" s="4"/>
       <c r="X24" s="5">
-        <v>1523</v>
+        <v>2596</v>
       </c>
       <c r="Y24" s="4"/>
       <c r="Z24" s="5">
-        <v>1524</v>
+        <v>2594</v>
       </c>
       <c r="AA24" s="4"/>
       <c r="AB24" s="5">
-        <v>2431</v>
+        <v>2595</v>
       </c>
       <c r="AC24" s="4"/>
       <c r="AD24" s="5">
-        <v>2432</v>
+        <v>790</v>
       </c>
       <c r="AE24" s="4"/>
       <c r="AF24" s="5">
-        <v>997</v>
+        <v>1471</v>
       </c>
       <c r="AG24" s="4"/>
       <c r="AH24" s="5">
-        <v>887</v>
+        <v>194</v>
       </c>
       <c r="AI24" s="4"/>
     </row>
-    <row r="25" spans="1:35" ht="25.15" customHeight="1">
+    <row r="25" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="5">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="5">
-        <v>2470</v>
+        <v>1027</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="5">
-        <v>2472</v>
+        <v>1029</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="5">
-        <v>2421</v>
+        <v>1544</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="5">
-        <v>380</v>
+        <v>2610</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="5">
-        <v>721</v>
+        <v>1018</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="5">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="P25" s="4"/>
-      <c r="Q25" s="5" t="s">
-        <v>48</v>
+      <c r="Q25" s="5">
+        <v>1013</v>
       </c>
       <c r="R25" s="4"/>
       <c r="S25" s="5">
-        <v>321</v>
+        <v>1010</v>
       </c>
       <c r="T25" s="4"/>
-      <c r="U25" s="5">
-        <v>586</v>
+      <c r="U25" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="V25" s="4"/>
       <c r="W25" s="5">
-        <v>2508</v>
+        <v>710</v>
       </c>
       <c r="X25" s="4"/>
-      <c r="Y25" s="5" t="s">
-        <v>49</v>
+      <c r="Y25" s="5">
+        <v>2593</v>
       </c>
       <c r="Z25" s="4"/>
       <c r="AA25" s="5">
-        <v>703</v>
+        <v>2592</v>
       </c>
       <c r="AB25" s="4"/>
       <c r="AC25" s="5">
-        <v>411</v>
+        <v>1441</v>
       </c>
       <c r="AD25" s="4"/>
       <c r="AE25" s="5">
-        <v>1801</v>
+        <v>793</v>
       </c>
       <c r="AF25" s="4"/>
       <c r="AG25" s="5">
-        <v>1851</v>
+        <v>1473</v>
       </c>
       <c r="AH25" s="4"/>
       <c r="AI25" s="5">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" ht="25.15" customHeight="1">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B26" s="5">
-        <v>1023</v>
+        <v>2651</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="5">
-        <v>1026</v>
+        <v>2567</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="5">
-        <v>1028</v>
+        <v>2566</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="5">
-        <v>1030</v>
+        <v>1067</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="5">
-        <v>598</v>
+        <v>2420</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="5">
-        <v>1017</v>
+        <v>883</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="5">
-        <v>1021</v>
+        <v>884</v>
       </c>
       <c r="O26" s="4"/>
-      <c r="P26" s="5" t="s">
-        <v>51</v>
+      <c r="P26" s="5">
+        <v>1014</v>
       </c>
       <c r="Q26" s="4"/>
       <c r="R26" s="5">
-        <v>1008</v>
+        <v>1015</v>
       </c>
       <c r="S26" s="4"/>
       <c r="T26" s="5">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="U26" s="4"/>
       <c r="V26" s="5">
-        <v>2483</v>
+        <v>709</v>
       </c>
       <c r="W26" s="4"/>
       <c r="X26" s="5">
-        <v>2596</v>
+        <v>712</v>
       </c>
       <c r="Y26" s="4"/>
       <c r="Z26" s="5">
-        <v>2594</v>
+        <v>2591</v>
       </c>
       <c r="AA26" s="4"/>
       <c r="AB26" s="5">
-        <v>2595</v>
+        <v>1440</v>
       </c>
       <c r="AC26" s="4"/>
-      <c r="AD26" s="5">
-        <v>790</v>
+      <c r="AD26" s="6">
+        <v>792</v>
       </c>
       <c r="AE26" s="4"/>
       <c r="AF26" s="5">
-        <v>1471</v>
+        <v>1474</v>
       </c>
       <c r="AG26" s="4"/>
       <c r="AH26" s="5">
-        <v>194</v>
+        <v>1475</v>
       </c>
       <c r="AI26" s="4"/>
     </row>
-    <row r="27" spans="1:35" ht="25.15" customHeight="1">
+    <row r="27" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="5">
-        <v>1024</v>
+        <v>344</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="5">
-        <v>1027</v>
+        <v>2568</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="5">
-        <v>1029</v>
+        <v>271</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="5">
-        <v>1544</v>
+        <v>241</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="5">
-        <v>2610</v>
+        <v>226</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="5">
-        <v>1018</v>
+        <v>596</v>
       </c>
       <c r="N27" s="4"/>
       <c r="O27" s="5">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="5">
-        <v>1013</v>
+        <v>1016</v>
       </c>
       <c r="R27" s="4"/>
       <c r="S27" s="5">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="T27" s="4"/>
-      <c r="U27" s="5" t="s">
-        <v>53</v>
+      <c r="U27" s="5">
+        <v>711</v>
       </c>
       <c r="V27" s="4"/>
       <c r="W27" s="5">
-        <v>710</v>
+        <v>199</v>
       </c>
       <c r="X27" s="4"/>
-      <c r="Y27" s="5">
-        <v>2593</v>
+      <c r="Y27" s="7">
+        <v>2213</v>
       </c>
       <c r="Z27" s="4"/>
       <c r="AA27" s="5">
-        <v>2592</v>
+        <v>823</v>
       </c>
       <c r="AB27" s="4"/>
       <c r="AC27" s="5">
-        <v>1441</v>
+        <v>2218</v>
       </c>
       <c r="AD27" s="4"/>
       <c r="AE27" s="5">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="AF27" s="4"/>
       <c r="AG27" s="5">
-        <v>1473</v>
+        <v>1476</v>
       </c>
       <c r="AH27" s="4"/>
       <c r="AI27" s="5">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="28" spans="1:35" ht="25.15" customHeight="1">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B28" s="5">
-        <v>2651</v>
+        <v>1066</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="5">
-        <v>2567</v>
+        <v>354</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="5">
-        <v>2566</v>
+      <c r="F28" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="5">
-        <v>1067</v>
+        <v>1</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="5">
-        <v>2420</v>
+        <v>1734</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="5">
-        <v>883</v>
+        <v>308</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="5">
-        <v>884</v>
+        <v>1170</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="5">
-        <v>1014</v>
+        <v>2299</v>
       </c>
       <c r="Q28" s="4"/>
       <c r="R28" s="5">
-        <v>1015</v>
+        <v>1415</v>
       </c>
       <c r="S28" s="4"/>
       <c r="T28" s="5">
-        <v>1011</v>
+        <v>618</v>
       </c>
       <c r="U28" s="4"/>
       <c r="V28" s="5">
-        <v>709</v>
+        <v>719</v>
       </c>
       <c r="W28" s="4"/>
       <c r="X28" s="5">
-        <v>712</v>
+        <v>720</v>
       </c>
       <c r="Y28" s="4"/>
       <c r="Z28" s="5">
-        <v>2591</v>
+        <v>824</v>
       </c>
       <c r="AA28" s="4"/>
       <c r="AB28" s="5">
-        <v>1440</v>
+        <v>517</v>
       </c>
       <c r="AC28" s="4"/>
-      <c r="AD28" s="6">
-        <v>792</v>
+      <c r="AD28" s="5">
+        <v>794</v>
       </c>
       <c r="AE28" s="4"/>
       <c r="AF28" s="5">
-        <v>1474</v>
+        <v>740</v>
       </c>
       <c r="AG28" s="4"/>
       <c r="AH28" s="5">
-        <v>1475</v>
+        <v>1478</v>
       </c>
       <c r="AI28" s="4"/>
     </row>
-    <row r="29" spans="1:35" ht="25.15" customHeight="1">
+    <row r="29" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="5">
-        <v>344</v>
+        <v>1231</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="5">
-        <v>2568</v>
+        <v>2357</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="5">
-        <v>271</v>
+        <v>26</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="5">
-        <v>241</v>
+        <v>662</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="5">
-        <v>226</v>
+        <v>173</v>
       </c>
       <c r="L29" s="4"/>
       <c r="M29" s="5">
-        <v>596</v>
+        <v>1645</v>
       </c>
       <c r="N29" s="4"/>
       <c r="O29" s="5">
-        <v>1020</v>
+        <v>2298</v>
       </c>
       <c r="P29" s="4"/>
       <c r="Q29" s="5">
-        <v>1016</v>
+        <v>2301</v>
       </c>
       <c r="R29" s="4"/>
       <c r="S29" s="5">
-        <v>1012</v>
+        <v>1074</v>
       </c>
       <c r="T29" s="4"/>
       <c r="U29" s="5">
-        <v>711</v>
+        <v>1075</v>
       </c>
       <c r="V29" s="4"/>
       <c r="W29" s="5">
-        <v>199</v>
+        <v>1042</v>
       </c>
       <c r="X29" s="4"/>
-      <c r="Y29" s="7">
-        <v>2213</v>
+      <c r="Y29" s="5">
+        <v>1043</v>
       </c>
       <c r="Z29" s="4"/>
       <c r="AA29" s="5">
-        <v>823</v>
+        <v>1044</v>
       </c>
       <c r="AB29" s="4"/>
       <c r="AC29" s="5">
-        <v>2218</v>
+        <v>1045</v>
       </c>
       <c r="AD29" s="4"/>
       <c r="AE29" s="5">
-        <v>791</v>
+        <v>1602</v>
       </c>
       <c r="AF29" s="4"/>
       <c r="AG29" s="5">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="AH29" s="4"/>
       <c r="AI29" s="5">
-        <v>1479</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35" ht="25.15" customHeight="1">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B30" s="5">
-        <v>1066</v>
+        <v>19</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="5">
-        <v>354</v>
+        <v>2475</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="5" t="s">
-        <v>57</v>
+      <c r="F30" s="5">
+        <v>2479</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="5">
-        <v>1</v>
+        <v>2331</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="5">
-        <v>1734</v>
+        <v>2333</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="5">
-        <v>308</v>
+        <v>2330</v>
       </c>
       <c r="M30" s="4"/>
-      <c r="N30" s="5">
-        <v>1170</v>
+      <c r="N30" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="5">
-        <v>2299</v>
+        <v>2300</v>
       </c>
       <c r="Q30" s="4"/>
       <c r="R30" s="5">
-        <v>1415</v>
+        <v>682</v>
       </c>
       <c r="S30" s="4"/>
       <c r="T30" s="5">
-        <v>618</v>
+        <v>1227</v>
       </c>
       <c r="U30" s="4"/>
       <c r="V30" s="5">
-        <v>719</v>
+        <v>143</v>
       </c>
       <c r="W30" s="4"/>
       <c r="X30" s="5">
-        <v>720</v>
+        <v>2284</v>
       </c>
       <c r="Y30" s="4"/>
       <c r="Z30" s="5">
-        <v>824</v>
+        <v>2285</v>
       </c>
       <c r="AA30" s="4"/>
-      <c r="AB30" s="5">
-        <v>517</v>
+      <c r="AB30" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="AC30" s="4"/>
       <c r="AD30" s="5">
-        <v>794</v>
+        <v>1534</v>
       </c>
       <c r="AE30" s="4"/>
       <c r="AF30" s="5">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="AG30" s="4"/>
       <c r="AH30" s="5">
-        <v>1478</v>
+        <v>2409</v>
       </c>
       <c r="AI30" s="4"/>
     </row>
-    <row r="31" spans="1:35" ht="25.15" customHeight="1">
+    <row r="31" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="5">
-        <v>1231</v>
+        <v>2474</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="5">
-        <v>2357</v>
+        <v>2478</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="5">
-        <v>26</v>
+        <v>2480</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="5">
-        <v>662</v>
+        <v>2332</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="5">
-        <v>173</v>
+        <v>2334</v>
       </c>
       <c r="L31" s="4"/>
       <c r="M31" s="5">
-        <v>1645</v>
+        <v>2521</v>
       </c>
       <c r="N31" s="4"/>
-      <c r="O31" s="5">
-        <v>2298</v>
+      <c r="O31" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="5">
-        <v>2301</v>
+        <v>2302</v>
       </c>
       <c r="R31" s="4"/>
       <c r="S31" s="5">
-        <v>1074</v>
+        <v>674</v>
       </c>
       <c r="T31" s="4"/>
       <c r="U31" s="5">
-        <v>1075</v>
+        <v>675</v>
       </c>
       <c r="V31" s="4"/>
       <c r="W31" s="5">
-        <v>1042</v>
+        <v>2208</v>
       </c>
       <c r="X31" s="4"/>
       <c r="Y31" s="5">
-        <v>1043</v>
+        <v>1092</v>
       </c>
       <c r="Z31" s="4"/>
       <c r="AA31" s="5">
-        <v>1044</v>
+        <v>1033</v>
       </c>
       <c r="AB31" s="4"/>
       <c r="AC31" s="5">
-        <v>1045</v>
+        <v>1032</v>
       </c>
       <c r="AD31" s="4"/>
       <c r="AE31" s="5">
-        <v>1602</v>
+        <v>1031</v>
       </c>
       <c r="AF31" s="4"/>
-      <c r="AG31" s="5">
-        <v>1477</v>
+      <c r="AG31" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="AH31" s="4"/>
       <c r="AI31" s="5">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="32" spans="1:35" ht="25.15" customHeight="1">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="32" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B32" s="5">
-        <v>19</v>
+        <v>2476</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="5">
-        <v>2475</v>
+        <v>2477</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="5">
-        <v>2479</v>
+        <v>2481</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="5">
-        <v>2331</v>
+        <v>2464</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="5">
-        <v>2333</v>
+        <v>121</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="5">
-        <v>2330</v>
+        <v>2613</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="5" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="5">
-        <v>2300</v>
+        <v>1520</v>
       </c>
       <c r="Q32" s="4"/>
       <c r="R32" s="5">
-        <v>682</v>
+        <v>208</v>
       </c>
       <c r="S32" s="4"/>
       <c r="T32" s="5">
-        <v>1227</v>
+        <v>207</v>
       </c>
       <c r="U32" s="4"/>
       <c r="V32" s="5">
-        <v>143</v>
+        <v>2205</v>
       </c>
       <c r="W32" s="4"/>
       <c r="X32" s="5">
-        <v>2284</v>
+        <v>2206</v>
       </c>
       <c r="Y32" s="4"/>
       <c r="Z32" s="5">
-        <v>2285</v>
+        <v>2212</v>
       </c>
       <c r="AA32" s="4"/>
-      <c r="AB32" s="5" t="s">
-        <v>61</v>
+      <c r="AB32" s="5">
+        <v>1034</v>
       </c>
       <c r="AC32" s="4"/>
       <c r="AD32" s="5">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="AE32" s="4"/>
       <c r="AF32" s="5">
-        <v>739</v>
+        <v>2590</v>
       </c>
       <c r="AG32" s="4"/>
-      <c r="AH32" s="5">
-        <v>2409</v>
+      <c r="AH32" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="AI32" s="4"/>
     </row>
-    <row r="33" spans="1:35" ht="25.15" customHeight="1">
+    <row r="33" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="5">
-        <v>2474</v>
+        <v>155</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="5">
-        <v>2478</v>
+        <v>2401</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="5">
-        <v>2480</v>
+        <v>245</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="5">
-        <v>2332</v>
+        <v>602</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="5">
-        <v>2334</v>
+        <v>2441</v>
       </c>
       <c r="L33" s="4"/>
-      <c r="M33" s="5">
-        <v>2521</v>
+      <c r="M33" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="N33" s="4"/>
       <c r="O33" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="P33" s="4"/>
       <c r="Q33" s="5">
-        <v>2302</v>
+        <v>1038</v>
       </c>
       <c r="R33" s="4"/>
       <c r="S33" s="5">
-        <v>674</v>
+        <v>1039</v>
       </c>
       <c r="T33" s="4"/>
       <c r="U33" s="5">
-        <v>675</v>
+        <v>1041</v>
       </c>
       <c r="V33" s="4"/>
       <c r="W33" s="5">
-        <v>2208</v>
+        <v>2204</v>
       </c>
       <c r="X33" s="4"/>
       <c r="Y33" s="5">
-        <v>1092</v>
+        <v>1798</v>
       </c>
       <c r="Z33" s="4"/>
       <c r="AA33" s="5">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="AB33" s="4"/>
       <c r="AC33" s="5">
-        <v>1032</v>
+        <v>1036</v>
       </c>
       <c r="AD33" s="4"/>
-      <c r="AE33" s="5">
-        <v>1031</v>
+      <c r="AE33" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="AF33" s="4"/>
       <c r="AG33" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="AH33" s="4"/>
-      <c r="AI33" s="5">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="34" spans="1:35" ht="25.15" customHeight="1">
+      <c r="AI33" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B34" s="5">
-        <v>2476</v>
+        <v>2029</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="5">
-        <v>2477</v>
+        <v>1050</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="5">
-        <v>2481</v>
+        <v>1051</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="5">
-        <v>2464</v>
+        <v>1052</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="5">
-        <v>121</v>
+        <v>1053</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="5">
-        <v>2613</v>
+        <v>2447</v>
       </c>
       <c r="M34" s="4"/>
-      <c r="N34" s="5" t="s">
-        <v>66</v>
+      <c r="N34" s="5">
+        <v>2653</v>
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="5">
-        <v>1520</v>
+        <v>2654</v>
       </c>
       <c r="Q34" s="4"/>
       <c r="R34" s="5">
-        <v>208</v>
+        <v>1040</v>
       </c>
       <c r="S34" s="4"/>
       <c r="T34" s="5">
-        <v>207</v>
+        <v>1037</v>
       </c>
       <c r="U34" s="4"/>
       <c r="V34" s="5">
-        <v>2205</v>
+        <v>1049</v>
       </c>
       <c r="W34" s="4"/>
       <c r="X34" s="5">
-        <v>2206</v>
+        <v>1799</v>
       </c>
       <c r="Y34" s="4"/>
       <c r="Z34" s="5">
-        <v>2212</v>
+        <v>1797</v>
       </c>
       <c r="AA34" s="4"/>
       <c r="AB34" s="5">
-        <v>1034</v>
+        <v>981</v>
       </c>
       <c r="AC34" s="4"/>
       <c r="AD34" s="5">
-        <v>1535</v>
+        <v>1908</v>
       </c>
       <c r="AE34" s="4"/>
-      <c r="AF34" s="5">
-        <v>2590</v>
+      <c r="AF34" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="AG34" s="4"/>
       <c r="AH34" s="5" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="AI34" s="4"/>
     </row>
-    <row r="35" spans="1:35" ht="25.15" customHeight="1">
+    <row r="35" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="5">
-        <v>155</v>
+        <v>1632</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="5">
-        <v>2401</v>
+        <v>1442</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="5">
-        <v>245</v>
+        <v>2615</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="5">
-        <v>602</v>
+        <v>2451</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="5">
-        <v>2441</v>
+        <v>1778</v>
       </c>
       <c r="L35" s="4"/>
-      <c r="M35" s="5" t="s">
-        <v>69</v>
+      <c r="M35" s="5">
+        <v>2429</v>
       </c>
       <c r="N35" s="4"/>
-      <c r="O35" s="5" t="s">
-        <v>70</v>
+      <c r="O35" s="5">
+        <v>2531</v>
       </c>
       <c r="P35" s="4"/>
       <c r="Q35" s="5">
-        <v>1038</v>
+        <v>2532</v>
       </c>
       <c r="R35" s="4"/>
       <c r="S35" s="5">
-        <v>1039</v>
+        <v>2374</v>
       </c>
       <c r="T35" s="4"/>
       <c r="U35" s="5">
-        <v>1041</v>
+        <v>1048</v>
       </c>
       <c r="V35" s="4"/>
       <c r="W35" s="5">
-        <v>2204</v>
+        <v>1046</v>
       </c>
       <c r="X35" s="4"/>
       <c r="Y35" s="5">
-        <v>1798</v>
+        <v>1542</v>
       </c>
       <c r="Z35" s="4"/>
       <c r="AA35" s="5">
-        <v>1035</v>
+        <v>982</v>
       </c>
       <c r="AB35" s="4"/>
       <c r="AC35" s="5">
-        <v>1036</v>
+        <v>2257</v>
       </c>
       <c r="AD35" s="4"/>
       <c r="AE35" s="5" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="AF35" s="4"/>
       <c r="AG35" s="5" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="AH35" s="4"/>
       <c r="AI35" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:35" ht="25.15" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B36" s="5">
-        <v>2029</v>
+        <v>1068</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="5">
-        <v>1050</v>
+        <v>1069</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="5">
-        <v>1051</v>
+        <v>238</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="5">
-        <v>1052</v>
+        <v>298</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="5">
-        <v>1053</v>
+        <v>1072</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="5">
-        <v>2447</v>
+        <v>2426</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="5">
-        <v>2653</v>
+        <v>2427</v>
       </c>
       <c r="O36" s="4"/>
       <c r="P36" s="5">
-        <v>2654</v>
+        <v>2428</v>
       </c>
       <c r="Q36" s="4"/>
-      <c r="R36" s="5">
-        <v>1040</v>
+      <c r="R36" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="S36" s="4"/>
       <c r="T36" s="5">
-        <v>1037</v>
+        <v>2657</v>
       </c>
       <c r="U36" s="4"/>
       <c r="V36" s="5">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="W36" s="4"/>
       <c r="X36" s="5">
-        <v>1799</v>
+        <v>15</v>
       </c>
       <c r="Y36" s="4"/>
       <c r="Z36" s="5">
-        <v>1797</v>
+        <v>16</v>
       </c>
       <c r="AA36" s="4"/>
       <c r="AB36" s="5">
-        <v>981</v>
+        <v>2258</v>
       </c>
       <c r="AC36" s="4"/>
       <c r="AD36" s="5">
-        <v>1908</v>
+        <v>82</v>
       </c>
       <c r="AE36" s="4"/>
       <c r="AF36" s="5" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="AG36" s="4"/>
       <c r="AH36" s="5" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI36" s="4"/>
     </row>
-    <row r="37" spans="1:35" ht="25.15" customHeight="1">
+    <row r="37" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="5">
-        <v>1632</v>
+        <v>922</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="5">
-        <v>1442</v>
+        <v>1584</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="5">
-        <v>2615</v>
+        <v>1190</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="5">
-        <v>2451</v>
+        <v>1191</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="5">
-        <v>1778</v>
+        <v>2320</v>
       </c>
       <c r="L37" s="4"/>
       <c r="M37" s="5">
-        <v>2429</v>
+        <v>1902</v>
       </c>
       <c r="N37" s="4"/>
       <c r="O37" s="5">
-        <v>2531</v>
+        <v>2547</v>
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" s="5">
-        <v>2532</v>
+        <v>1178</v>
       </c>
       <c r="R37" s="4"/>
       <c r="S37" s="5">
-        <v>2374</v>
+        <v>1938</v>
       </c>
       <c r="T37" s="4"/>
       <c r="U37" s="5">
-        <v>1048</v>
+        <v>1939</v>
       </c>
       <c r="V37" s="4"/>
       <c r="W37" s="5">
-        <v>1046</v>
+        <v>1080</v>
       </c>
       <c r="X37" s="4"/>
       <c r="Y37" s="5">
-        <v>1542</v>
+        <v>2380</v>
       </c>
       <c r="Z37" s="4"/>
       <c r="AA37" s="5">
-        <v>982</v>
+        <v>2677</v>
       </c>
       <c r="AB37" s="4"/>
       <c r="AC37" s="5">
-        <v>2257</v>
+        <v>2678</v>
       </c>
       <c r="AD37" s="4"/>
       <c r="AE37" s="5" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="AF37" s="4"/>
       <c r="AG37" s="5" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="AH37" s="4"/>
       <c r="AI37" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:35" ht="25.15" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B38" s="5">
-        <v>1068</v>
+        <v>1489</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="5">
-        <v>1069</v>
+        <v>1642</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="5">
-        <v>238</v>
+        <v>701</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="5">
-        <v>298</v>
+        <v>2415</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="5">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="5">
-        <v>2426</v>
+        <v>2660</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="5">
-        <v>2427</v>
+        <v>570</v>
       </c>
       <c r="O38" s="4"/>
       <c r="P38" s="5">
-        <v>2428</v>
+        <v>1818</v>
       </c>
       <c r="Q38" s="4"/>
-      <c r="R38" s="5" t="s">
-        <v>82</v>
+      <c r="R38" s="5">
+        <v>1940</v>
       </c>
       <c r="S38" s="4"/>
       <c r="T38" s="5">
-        <v>2657</v>
+        <v>1941</v>
       </c>
       <c r="U38" s="4"/>
-      <c r="V38" s="5">
-        <v>1047</v>
+      <c r="V38" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="W38" s="4"/>
       <c r="X38" s="5">
-        <v>15</v>
+        <v>557</v>
       </c>
       <c r="Y38" s="4"/>
       <c r="Z38" s="5">
-        <v>16</v>
+        <v>558</v>
       </c>
       <c r="AA38" s="4"/>
       <c r="AB38" s="5">
-        <v>2258</v>
+        <v>2676</v>
       </c>
       <c r="AC38" s="4"/>
       <c r="AD38" s="5">
-        <v>82</v>
+        <v>1579</v>
       </c>
       <c r="AE38" s="4"/>
       <c r="AF38" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AG38" s="4"/>
       <c r="AH38" s="5" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="AI38" s="4"/>
     </row>
-    <row r="39" spans="1:35" ht="25.15" customHeight="1">
+    <row r="39" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="5">
-        <v>922</v>
+        <v>13</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="5">
-        <v>1584</v>
+        <v>240</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="5">
-        <v>1190</v>
+        <v>200</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="5">
-        <v>1191</v>
+        <v>347</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="5">
-        <v>2320</v>
+        <v>475</v>
       </c>
       <c r="L39" s="4"/>
       <c r="M39" s="5">
-        <v>1902</v>
+        <v>2309</v>
       </c>
       <c r="N39" s="4"/>
       <c r="O39" s="5">
-        <v>2547</v>
+        <v>2395</v>
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="5">
-        <v>1178</v>
+        <v>202</v>
       </c>
       <c r="R39" s="4"/>
       <c r="S39" s="5">
-        <v>1938</v>
+        <v>2639</v>
       </c>
       <c r="T39" s="4"/>
       <c r="U39" s="5">
-        <v>1939</v>
+        <v>435</v>
       </c>
       <c r="V39" s="4"/>
       <c r="W39" s="5">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="X39" s="4"/>
       <c r="Y39" s="5">
-        <v>2380</v>
+        <v>1163</v>
       </c>
       <c r="Z39" s="4"/>
       <c r="AA39" s="5">
-        <v>2677</v>
+        <v>2679</v>
       </c>
       <c r="AB39" s="4"/>
       <c r="AC39" s="5">
-        <v>2678</v>
+        <v>2680</v>
       </c>
       <c r="AD39" s="4"/>
-      <c r="AE39" s="5" t="s">
-        <v>86</v>
+      <c r="AE39" s="5">
+        <v>1450</v>
       </c>
       <c r="AF39" s="4"/>
       <c r="AG39" s="5" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="AH39" s="4"/>
       <c r="AI39" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:35" ht="25.15" customHeight="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B40" s="5">
-        <v>1489</v>
+        <v>2444</v>
       </c>
       <c r="C40" s="4"/>
-      <c r="D40" s="5">
-        <v>1642</v>
+      <c r="D40" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="5">
-        <v>701</v>
+        <v>622</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="5">
-        <v>2415</v>
+        <v>1974</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="5">
-        <v>1073</v>
+        <v>2402</v>
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="5">
-        <v>2660</v>
+        <v>67</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="5">
-        <v>570</v>
+        <v>579</v>
       </c>
       <c r="O40" s="4"/>
       <c r="P40" s="5">
-        <v>1818</v>
+        <v>2459</v>
       </c>
       <c r="Q40" s="4"/>
       <c r="R40" s="5">
-        <v>1940</v>
+        <v>445</v>
       </c>
       <c r="S40" s="4"/>
       <c r="T40" s="5">
-        <v>1941</v>
+        <v>2620</v>
       </c>
       <c r="U40" s="4"/>
-      <c r="V40" s="5" t="s">
-        <v>90</v>
+      <c r="V40" s="5">
+        <v>1084</v>
       </c>
       <c r="W40" s="4"/>
       <c r="X40" s="5">
-        <v>557</v>
+        <v>576</v>
       </c>
       <c r="Y40" s="4"/>
       <c r="Z40" s="5">
-        <v>558</v>
+        <v>1152</v>
       </c>
       <c r="AA40" s="4"/>
       <c r="AB40" s="5">
-        <v>2676</v>
+        <v>854</v>
       </c>
       <c r="AC40" s="4"/>
       <c r="AD40" s="5">
-        <v>1579</v>
+        <v>855</v>
       </c>
       <c r="AE40" s="4"/>
       <c r="AF40" s="5" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="AG40" s="4"/>
       <c r="AH40" s="5" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="AI40" s="4"/>
     </row>
-    <row r="41" spans="1:35" ht="25.15" customHeight="1">
+    <row r="41" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B41" s="4"/>
-      <c r="C41" s="5">
-        <v>13</v>
+      <c r="C41" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="5">
-        <v>240</v>
+      <c r="E41" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="F41" s="4"/>
-      <c r="G41" s="5">
-        <v>200</v>
+      <c r="G41" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="5">
-        <v>347</v>
+        <v>18</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="5">
-        <v>475</v>
+        <v>259</v>
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="5">
-        <v>2309</v>
+        <v>2466</v>
       </c>
       <c r="N41" s="4"/>
       <c r="O41" s="5">
-        <v>2395</v>
+        <v>1904</v>
       </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="5">
-        <v>202</v>
+        <v>2488</v>
       </c>
       <c r="R41" s="4"/>
       <c r="S41" s="5">
-        <v>2639</v>
+        <v>2519</v>
       </c>
       <c r="T41" s="4"/>
       <c r="U41" s="5">
-        <v>435</v>
+        <v>2050</v>
       </c>
       <c r="V41" s="4"/>
       <c r="W41" s="5">
-        <v>1081</v>
+        <v>221</v>
       </c>
       <c r="X41" s="4"/>
       <c r="Y41" s="5">
-        <v>1163</v>
+        <v>76</v>
       </c>
       <c r="Z41" s="4"/>
       <c r="AA41" s="5">
-        <v>2679</v>
+        <v>1417</v>
       </c>
       <c r="AB41" s="4"/>
       <c r="AC41" s="5">
-        <v>2680</v>
+        <v>309</v>
       </c>
       <c r="AD41" s="4"/>
       <c r="AE41" s="5">
-        <v>1450</v>
+        <v>1502</v>
       </c>
       <c r="AF41" s="4"/>
-      <c r="AG41" s="5" t="s">
-        <v>94</v>
+      <c r="AG41" s="5">
+        <v>1817</v>
       </c>
       <c r="AH41" s="4"/>
-      <c r="AI41" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:35" ht="25.15" customHeight="1">
+      <c r="AI41" s="5">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="42" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B42" s="5">
-        <v>2444</v>
+        <v>1638</v>
       </c>
       <c r="C42" s="4"/>
-      <c r="D42" s="5" t="s">
-        <v>97</v>
+      <c r="D42" s="5">
+        <v>1852</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="5">
-        <v>622</v>
+        <v>2501</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5">
-        <v>1974</v>
+        <v>395</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="5">
-        <v>2402</v>
+        <v>1654</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="5">
-        <v>67</v>
+        <v>187</v>
       </c>
       <c r="M42" s="4"/>
       <c r="N42" s="5">
-        <v>579</v>
+        <v>1835</v>
       </c>
       <c r="O42" s="4"/>
       <c r="P42" s="5">
-        <v>2459</v>
+        <v>2543</v>
       </c>
       <c r="Q42" s="4"/>
       <c r="R42" s="5">
-        <v>445</v>
+        <v>2544</v>
       </c>
       <c r="S42" s="4"/>
       <c r="T42" s="5">
-        <v>2620</v>
+        <v>1087</v>
       </c>
       <c r="U42" s="4"/>
       <c r="V42" s="5">
-        <v>1084</v>
+        <v>1134</v>
       </c>
       <c r="W42" s="4"/>
       <c r="X42" s="5">
-        <v>576</v>
+        <v>2413</v>
       </c>
       <c r="Y42" s="4"/>
       <c r="Z42" s="5">
-        <v>1152</v>
+        <v>1596</v>
       </c>
       <c r="AA42" s="4"/>
       <c r="AB42" s="5">
-        <v>854</v>
+        <v>563</v>
       </c>
       <c r="AC42" s="4"/>
-      <c r="AD42" s="5">
-        <v>855</v>
+      <c r="AD42" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="AE42" s="4"/>
-      <c r="AF42" s="5" t="s">
-        <v>98</v>
+      <c r="AF42" s="5">
+        <v>306</v>
       </c>
       <c r="AG42" s="4"/>
-      <c r="AH42" s="5" t="s">
-        <v>99</v>
+      <c r="AH42" s="5">
+        <v>1214</v>
       </c>
       <c r="AI42" s="4"/>
     </row>
-    <row r="43" spans="1:35" ht="25.15" customHeight="1">
+    <row r="43" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B43" s="4"/>
-      <c r="C43" s="5" t="s">
-        <v>101</v>
+      <c r="C43" s="5">
+        <v>798</v>
       </c>
       <c r="D43" s="4"/>
-      <c r="E43" s="5" t="s">
-        <v>102</v>
+      <c r="E43" s="5">
+        <v>1206</v>
       </c>
       <c r="F43" s="4"/>
-      <c r="G43" s="5" t="s">
-        <v>103</v>
+      <c r="G43" s="5">
+        <v>2631</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="5">
-        <v>18</v>
+        <v>2407</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="5">
-        <v>259</v>
+        <v>1056</v>
       </c>
       <c r="L43" s="4"/>
       <c r="M43" s="5">
-        <v>2466</v>
+        <v>228</v>
       </c>
       <c r="N43" s="4"/>
       <c r="O43" s="5">
-        <v>1904</v>
+        <v>708</v>
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="5">
-        <v>2488</v>
+        <v>1877</v>
       </c>
       <c r="R43" s="4"/>
       <c r="S43" s="5">
-        <v>2519</v>
+        <v>22</v>
       </c>
       <c r="T43" s="4"/>
       <c r="U43" s="5">
-        <v>2050</v>
+        <v>246</v>
       </c>
       <c r="V43" s="4"/>
       <c r="W43" s="5">
-        <v>221</v>
+        <v>425</v>
       </c>
       <c r="X43" s="4"/>
       <c r="Y43" s="5">
-        <v>76</v>
+        <v>1841</v>
       </c>
       <c r="Z43" s="4"/>
       <c r="AA43" s="5">
-        <v>1417</v>
+        <v>2450</v>
       </c>
       <c r="AB43" s="4"/>
       <c r="AC43" s="5">
-        <v>309</v>
+        <v>2529</v>
       </c>
       <c r="AD43" s="4"/>
       <c r="AE43" s="5">
-        <v>1502</v>
+        <v>442</v>
       </c>
       <c r="AF43" s="4"/>
       <c r="AG43" s="5">
-        <v>1817</v>
+        <v>2599</v>
       </c>
       <c r="AH43" s="4"/>
       <c r="AI43" s="5">
-        <v>1621</v>
-      </c>
-    </row>
-    <row r="44" spans="1:35" ht="25.15" customHeight="1">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="44" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B44" s="5">
-        <v>1638</v>
+        <v>2303</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="5">
-        <v>1852</v>
+        <v>2551</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="5">
-        <v>2501</v>
-      </c>
+      <c r="F44" s="5"/>
       <c r="G44" s="4"/>
       <c r="H44" s="5">
-        <v>395</v>
+        <v>2618</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="5">
-        <v>1654</v>
+        <v>1110</v>
       </c>
       <c r="K44" s="4"/>
       <c r="L44" s="5">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="M44" s="4"/>
       <c r="N44" s="5">
-        <v>1835</v>
+        <v>2490</v>
       </c>
       <c r="O44" s="4"/>
       <c r="P44" s="5">
-        <v>2543</v>
+        <v>1136</v>
       </c>
       <c r="Q44" s="4"/>
       <c r="R44" s="5">
-        <v>2544</v>
+        <v>1062</v>
       </c>
       <c r="S44" s="4"/>
       <c r="T44" s="5">
-        <v>1087</v>
+        <v>451</v>
       </c>
       <c r="U44" s="4"/>
       <c r="V44" s="5">
-        <v>1134</v>
+        <v>190</v>
       </c>
       <c r="W44" s="4"/>
       <c r="X44" s="5">
-        <v>2413</v>
+        <v>78</v>
       </c>
       <c r="Y44" s="4"/>
       <c r="Z44" s="5">
-        <v>1596</v>
+        <v>1167</v>
       </c>
       <c r="AA44" s="4"/>
       <c r="AB44" s="5">
-        <v>563</v>
+        <v>1852</v>
       </c>
       <c r="AC44" s="4"/>
-      <c r="AD44" s="5" t="s">
-        <v>105</v>
+      <c r="AD44" s="5">
+        <v>623</v>
       </c>
       <c r="AE44" s="4"/>
       <c r="AF44" s="5">
-        <v>306</v>
+        <v>559</v>
       </c>
       <c r="AG44" s="4"/>
       <c r="AH44" s="5">
-        <v>1214</v>
+        <v>1897</v>
       </c>
       <c r="AI44" s="4"/>
     </row>
-    <row r="45" spans="1:35" ht="25.15" customHeight="1">
+    <row r="45" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="5">
-        <v>798</v>
+        <v>2642</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="5">
-        <v>1206</v>
+        <v>2406</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="5">
-        <v>2631</v>
+        <v>433</v>
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="5">
-        <v>2407</v>
+        <v>2662</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="5">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="5">
-        <v>228</v>
+        <v>80</v>
       </c>
       <c r="N45" s="4"/>
       <c r="O45" s="5">
-        <v>708</v>
+        <v>2656</v>
       </c>
       <c r="P45" s="4"/>
       <c r="Q45" s="5">
-        <v>1877</v>
+        <v>432</v>
       </c>
       <c r="R45" s="4"/>
       <c r="S45" s="5">
-        <v>22</v>
+        <v>1063</v>
       </c>
       <c r="T45" s="4"/>
       <c r="U45" s="5">
-        <v>246</v>
+        <v>396</v>
       </c>
       <c r="V45" s="4"/>
       <c r="W45" s="5">
-        <v>425</v>
+        <v>664</v>
       </c>
       <c r="X45" s="4"/>
       <c r="Y45" s="5">
-        <v>1841</v>
+        <v>416</v>
       </c>
       <c r="Z45" s="4"/>
       <c r="AA45" s="5">
-        <v>2450</v>
+        <v>2630</v>
       </c>
       <c r="AB45" s="4"/>
       <c r="AC45" s="5">
-        <v>2529</v>
+        <v>1496</v>
       </c>
       <c r="AD45" s="4"/>
       <c r="AE45" s="5">
-        <v>442</v>
+        <v>2335</v>
       </c>
       <c r="AF45" s="4"/>
       <c r="AG45" s="5">
-        <v>2599</v>
+        <v>2600</v>
       </c>
       <c r="AH45" s="4"/>
       <c r="AI45" s="5">
-        <v>1922</v>
-      </c>
-    </row>
-    <row r="46" spans="1:35" ht="25.15" customHeight="1">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="46" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B46" s="5">
-        <v>2303</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5">
-        <v>2551</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="4"/>
+        <v>760</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="5">
+        <v>2534</v>
+      </c>
+      <c r="G46" s="8"/>
       <c r="H46" s="5">
-        <v>2618</v>
-      </c>
-      <c r="I46" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="I46" s="8"/>
       <c r="J46" s="5">
-        <v>1110</v>
-      </c>
-      <c r="K46" s="4"/>
+        <v>225</v>
+      </c>
+      <c r="K46" s="8"/>
       <c r="L46" s="5">
-        <v>201</v>
-      </c>
-      <c r="M46" s="4"/>
+        <v>278</v>
+      </c>
+      <c r="M46" s="8"/>
       <c r="N46" s="5">
-        <v>2490</v>
-      </c>
-      <c r="O46" s="4"/>
+        <v>679</v>
+      </c>
+      <c r="O46" s="8"/>
       <c r="P46" s="5">
-        <v>1136</v>
-      </c>
-      <c r="Q46" s="4"/>
+        <v>2403</v>
+      </c>
+      <c r="Q46" s="8"/>
       <c r="R46" s="5">
-        <v>1062</v>
-      </c>
-      <c r="S46" s="4"/>
+        <v>1076</v>
+      </c>
+      <c r="S46" s="8"/>
       <c r="T46" s="5">
-        <v>451</v>
-      </c>
-      <c r="U46" s="4"/>
+        <v>1077</v>
+      </c>
+      <c r="U46" s="8"/>
       <c r="V46" s="5">
-        <v>190</v>
-      </c>
-      <c r="W46" s="4"/>
+        <v>176</v>
+      </c>
+      <c r="W46" s="8"/>
       <c r="X46" s="5">
-        <v>78</v>
-      </c>
-      <c r="Y46" s="4"/>
+        <v>2445</v>
+      </c>
+      <c r="Y46" s="8"/>
       <c r="Z46" s="5">
-        <v>1167</v>
-      </c>
-      <c r="AA46" s="4"/>
+        <v>2398</v>
+      </c>
+      <c r="AA46" s="8"/>
       <c r="AB46" s="5">
-        <v>1852</v>
-      </c>
-      <c r="AC46" s="4"/>
+        <v>2400</v>
+      </c>
+      <c r="AC46" s="8"/>
       <c r="AD46" s="5">
-        <v>623</v>
-      </c>
-      <c r="AE46" s="4"/>
+        <v>1157</v>
+      </c>
+      <c r="AE46" s="8"/>
       <c r="AF46" s="5">
-        <v>559</v>
-      </c>
-      <c r="AG46" s="4"/>
+        <v>1490</v>
+      </c>
+      <c r="AG46" s="8"/>
       <c r="AH46" s="5">
-        <v>1897</v>
-      </c>
-      <c r="AI46" s="4"/>
-    </row>
-    <row r="47" spans="1:35" ht="25.15" customHeight="1">
+        <v>2308</v>
+      </c>
+      <c r="AI46" s="8"/>
+    </row>
+    <row r="47" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="5">
-        <v>2642</v>
-      </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="5">
-        <v>2406</v>
-      </c>
-      <c r="F47" s="4"/>
-      <c r="G47" s="5">
-        <v>433</v>
-      </c>
-      <c r="H47" s="4"/>
-      <c r="I47" s="5">
-        <v>2662</v>
-      </c>
-      <c r="J47" s="4"/>
-      <c r="K47" s="5">
-        <v>1057</v>
-      </c>
-      <c r="L47" s="4"/>
-      <c r="M47" s="5">
-        <v>80</v>
-      </c>
-      <c r="N47" s="4"/>
-      <c r="O47" s="5">
-        <v>2656</v>
-      </c>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="5">
-        <v>432</v>
-      </c>
-      <c r="R47" s="4"/>
-      <c r="S47" s="5">
-        <v>1063</v>
-      </c>
-      <c r="T47" s="4"/>
-      <c r="U47" s="5">
-        <v>396</v>
-      </c>
-      <c r="V47" s="4"/>
-      <c r="W47" s="5">
-        <v>664</v>
-      </c>
-      <c r="X47" s="4"/>
-      <c r="Y47" s="5">
-        <v>416</v>
-      </c>
-      <c r="Z47" s="4"/>
-      <c r="AA47" s="5">
-        <v>2630</v>
-      </c>
-      <c r="AB47" s="4"/>
-      <c r="AC47" s="5">
-        <v>1496</v>
-      </c>
-      <c r="AD47" s="4"/>
-      <c r="AE47" s="5">
-        <v>2335</v>
-      </c>
-      <c r="AF47" s="4"/>
-      <c r="AG47" s="5">
-        <v>2600</v>
-      </c>
-      <c r="AH47" s="4"/>
-      <c r="AI47" s="5">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="48" spans="1:35" ht="25.15" customHeight="1">
-      <c r="A48" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B48" s="5">
-        <v>760</v>
-      </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="5">
-        <v>2534</v>
-      </c>
-      <c r="G48" s="8"/>
-      <c r="H48" s="5">
-        <v>103</v>
-      </c>
-      <c r="I48" s="8"/>
-      <c r="J48" s="5">
-        <v>225</v>
-      </c>
-      <c r="K48" s="8"/>
-      <c r="L48" s="5">
-        <v>278</v>
-      </c>
-      <c r="M48" s="8"/>
-      <c r="N48" s="5">
-        <v>679</v>
-      </c>
-      <c r="O48" s="8"/>
-      <c r="P48" s="5">
-        <v>2403</v>
-      </c>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="5">
-        <v>1076</v>
-      </c>
-      <c r="S48" s="8"/>
-      <c r="T48" s="5">
-        <v>1077</v>
-      </c>
-      <c r="U48" s="8"/>
-      <c r="V48" s="5">
-        <v>176</v>
-      </c>
-      <c r="W48" s="8"/>
-      <c r="X48" s="5">
-        <v>2445</v>
-      </c>
-      <c r="Y48" s="8"/>
-      <c r="Z48" s="5">
-        <v>2398</v>
-      </c>
-      <c r="AA48" s="8"/>
-      <c r="AB48" s="5">
-        <v>2400</v>
-      </c>
-      <c r="AC48" s="8"/>
-      <c r="AD48" s="5">
-        <v>1157</v>
-      </c>
-      <c r="AE48" s="8"/>
-      <c r="AF48" s="5">
-        <v>1490</v>
-      </c>
-      <c r="AG48" s="8"/>
-      <c r="AH48" s="5">
-        <v>2308</v>
-      </c>
-      <c r="AI48" s="8"/>
-    </row>
-    <row r="49" spans="1:35" ht="25.15" customHeight="1">
-      <c r="A49" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="9"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="9"/>
-      <c r="T49" s="8"/>
-      <c r="U49" s="9"/>
-      <c r="V49" s="8"/>
-      <c r="W49" s="9"/>
-      <c r="X49" s="8"/>
-      <c r="Y49" s="9"/>
-      <c r="Z49" s="8"/>
-      <c r="AA49" s="9"/>
-      <c r="AB49" s="8"/>
-      <c r="AC49" s="9"/>
-      <c r="AD49" s="8"/>
-      <c r="AE49" s="9"/>
-      <c r="AF49" s="8"/>
-      <c r="AG49" s="9"/>
-      <c r="AH49" s="8"/>
-      <c r="AI49" s="9"/>
-    </row>
-    <row r="55" spans="1:35">
-      <c r="B55" t="s">
-        <v>112</v>
-      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="8"/>
+      <c r="U47" s="9"/>
+      <c r="V47" s="8"/>
+      <c r="W47" s="9"/>
+      <c r="X47" s="8"/>
+      <c r="Y47" s="9"/>
+      <c r="Z47" s="8"/>
+      <c r="AA47" s="9"/>
+      <c r="AB47" s="8"/>
+      <c r="AC47" s="9"/>
+      <c r="AD47" s="8"/>
+      <c r="AE47" s="9"/>
+      <c r="AF47" s="8"/>
+      <c r="AG47" s="9"/>
+      <c r="AH47" s="8"/>
+      <c r="AI47" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4208,6 +4197,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <StockShowRelated xmlns="4816bd95-4284-4c65-a343-fbbfe3c79838">false</StockShowRelated>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4816bd95-4284-4c65-a343-fbbfe3c79838">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0f439937-ee6a-4379-a5d5-430fe2261004" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010081AD44C0CBEB304E93E820FB24B13251" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f73d017c857550f142d63a5bbe9cecd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4816bd95-4284-4c65-a343-fbbfe3c79838" xmlns:ns3="0f439937-ee6a-4379-a5d5-430fe2261004" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4bd163e8bb288cd9cbd6306fe34550d6" ns2:_="" ns3:_="">
     <xsd:import namespace="4816bd95-4284-4c65-a343-fbbfe3c79838"/>
@@ -4426,26 +4427,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <StockShowRelated xmlns="4816bd95-4284-4c65-a343-fbbfe3c79838">false</StockShowRelated>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4816bd95-4284-4c65-a343-fbbfe3c79838">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0f439937-ee6a-4379-a5d5-430fe2261004" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{781E94E0-BE5E-4E9A-AFB8-688BB9152370}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{781E94E0-BE5E-4E9A-AFB8-688BB9152370}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAF223EA-765A-40B2-BAE9-14CF812436E5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B7A1D37-FE14-4D67-9004-2725601C938F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4816bd95-4284-4c65-a343-fbbfe3c79838"/>
+    <ds:schemaRef ds:uri="0f439937-ee6a-4379-a5d5-430fe2261004"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B7A1D37-FE14-4D67-9004-2725601C938F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAF223EA-765A-40B2-BAE9-14CF812436E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4816bd95-4284-4c65-a343-fbbfe3c79838"/>
+    <ds:schemaRef ds:uri="0f439937-ee6a-4379-a5d5-430fe2261004"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>